<commit_message>
Fixed 2012 program specialities
Code was only accessing 2012 specialties till 'conservation and land use' had make an exception for 2012 in code. New code now includes all values
</commit_message>
<xml_diff>
--- a/program_specialties/program_specialties_2012.xlsx
+++ b/program_specialties/program_specialties_2012.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="9840" yWindow="45" windowWidth="10800" windowHeight="8445"/>
@@ -3625,7 +3625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC949"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="N35" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="D35" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AD50" sqref="AD50"/>
     </sheetView>
   </sheetViews>

</xml_diff>